<commit_message>
Modified webDriver Classed. These are now dynamic
</commit_message>
<xml_diff>
--- a/Resources/Config.xlsx
+++ b/Resources/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Timeout</t>
   </si>
@@ -48,10 +48,31 @@
     <t>TO crawl links on site</t>
   </si>
   <si>
-    <t>BWS siteURL</t>
-  </si>
-  <si>
-    <t>Url</t>
+    <t>ChromeServerLocation</t>
+  </si>
+  <si>
+    <t>PhantomJSLocation</t>
+  </si>
+  <si>
+    <t>Resources\servers\chromedriver.exe</t>
+  </si>
+  <si>
+    <t>Resources\servers\IEDriverServer.exe</t>
+  </si>
+  <si>
+    <t>Resources\servers\phantomjs.exe</t>
+  </si>
+  <si>
+    <t>ConfigDevUrl</t>
+  </si>
+  <si>
+    <t>ConfigDevUsername</t>
+  </si>
+  <si>
+    <t>ConfigDevPassword</t>
+  </si>
+  <si>
+    <t>IEServerLocation</t>
   </si>
 </sst>
 </file>
@@ -124,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -136,9 +157,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -447,16 +465,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,33 +523,48 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Basic auth support other than IE
</commit_message>
<xml_diff>
--- a/Resources/Config.xlsx
+++ b/Resources/Config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Timeout</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Value in second</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>ThreadsToCrawlSite</t>
   </si>
   <si>
@@ -73,6 +70,18 @@
   </si>
   <si>
     <t>IEServerLocation</t>
+  </si>
+  <si>
+    <t>http://bws-selfservice.unileversolutions.com/</t>
+  </si>
+  <si>
+    <t>skumar213@sapient.com</t>
+  </si>
+  <si>
+    <t>334512s</t>
+  </si>
+  <si>
+    <t>IE</t>
   </si>
 </sst>
 </file>
@@ -145,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,6 +172,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,7 +480,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
@@ -513,57 +525,65 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -572,8 +592,11 @@
       <formula1>"Firefox, Chrome, IE, Phantom"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>